<commit_message>
day_8 task of data validation has been completed
</commit_message>
<xml_diff>
--- a/European_Coaching/day_5/excel/task-2.xlsx
+++ b/European_Coaching/day_5/excel/task-2.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t xml:space="preserve">month </t>
   </si>
@@ -33,9 +32,6 @@
     <t>principle aomunt with rate</t>
   </si>
   <si>
-    <t>RD AMONUT</t>
-  </si>
-  <si>
     <t xml:space="preserve">MONTH </t>
   </si>
   <si>
@@ -52,6 +48,27 @@
   </si>
   <si>
     <t>YEAR</t>
+  </si>
+  <si>
+    <t>RD AMOUNT</t>
+  </si>
+  <si>
+    <t>OPENING BALNACE</t>
+  </si>
+  <si>
+    <t>PRINICPAL AMOUNT</t>
+  </si>
+  <si>
+    <t>INTEREST REATE 7.10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRINCIPAL AMOUNT WITH RATE </t>
+  </si>
+  <si>
+    <t>MONTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -125,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -139,6 +156,7 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,12 +519,12 @@
         <v>1000</v>
       </c>
       <c r="E5" s="4">
-        <f>SUM((C5+D5)*7.1%/12)</f>
-        <v>11.868340277777776</v>
+        <f>SUM((Sheet3!EC5+D5)*7.1%/12)</f>
+        <v>5.916666666666667</v>
       </c>
       <c r="F5" s="4">
         <f>SUM(C5:E5)</f>
-        <v>2017.7850069444444</v>
+        <v>2011.8333333333333</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -515,18 +533,18 @@
       </c>
       <c r="C6" s="4">
         <f t="shared" ref="C6:C21" si="0">F5</f>
-        <v>2017.7850069444444</v>
+        <v>2011.8333333333333</v>
       </c>
       <c r="D6" s="4">
         <v>1000</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" ref="E6:E21" si="1">SUM((C6+D6)*7.1%/12)</f>
-        <v>17.855227957754629</v>
+        <v>17.820013888888884</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" ref="F6:F21" si="2">SUM(C6:E6)</f>
-        <v>3035.6402349021992</v>
+        <v>3029.6533472222218</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -535,18 +553,18 @@
       </c>
       <c r="C7" s="4">
         <f t="shared" si="0"/>
-        <v>3035.6402349021992</v>
+        <v>3029.6533472222218</v>
       </c>
       <c r="D7" s="4">
         <v>1000</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="1"/>
-        <v>23.877538056504676</v>
+        <v>23.842115637731478</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="2"/>
-        <v>4059.517772958704</v>
+        <v>4053.4954628599535</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -555,18 +573,18 @@
       </c>
       <c r="C8" s="4">
         <f t="shared" si="0"/>
-        <v>4059.517772958704</v>
+        <v>4053.4954628599535</v>
       </c>
       <c r="D8" s="4">
         <v>1000</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="1"/>
-        <v>29.93548015667233</v>
+        <v>29.89984815525472</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="2"/>
-        <v>5089.4532531153764</v>
+        <v>5083.3953110152079</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -575,18 +593,18 @@
       </c>
       <c r="C9" s="4">
         <f t="shared" si="0"/>
-        <v>5089.4532531153764</v>
+        <v>5083.3953110152079</v>
       </c>
       <c r="D9" s="4">
         <v>1000</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="1"/>
-        <v>36.029265080932639</v>
+        <v>35.993422256839978</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="2"/>
-        <v>6125.4825181963088</v>
+        <v>6119.3887332720478</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -595,18 +613,18 @@
       </c>
       <c r="C10" s="4">
         <f t="shared" si="0"/>
-        <v>6125.4825181963088</v>
+        <v>6119.3887332720478</v>
       </c>
       <c r="D10" s="4">
         <v>1000</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="1"/>
-        <v>42.159104899328156</v>
+        <v>42.123050005192944</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
-        <v>7167.6416230956365</v>
+        <v>7161.5117832772412</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -615,18 +633,18 @@
       </c>
       <c r="C11" s="4">
         <f t="shared" si="0"/>
-        <v>7167.6416230956365</v>
+        <v>7161.5117832772412</v>
       </c>
       <c r="D11" s="4">
         <v>1000</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>48.325212936649173</v>
+        <v>48.288944717723673</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
-        <v>8215.9668360322848</v>
+        <v>8209.8007279949652</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -635,18 +653,18 @@
       </c>
       <c r="C12" s="4">
         <f t="shared" si="0"/>
-        <v>8215.9668360322848</v>
+        <v>8209.8007279949652</v>
       </c>
       <c r="D12" s="4">
         <v>1000</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="1"/>
-        <v>54.527803779857685</v>
+        <v>54.491320973970204</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
-        <v>9270.4946398121429</v>
+        <v>9264.292048968935</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -655,18 +673,18 @@
       </c>
       <c r="C13" s="4">
         <f t="shared" si="0"/>
-        <v>9270.4946398121429</v>
+        <v>9264.292048968935</v>
       </c>
       <c r="D13" s="4">
         <v>1000</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="1"/>
-        <v>60.767093285555177</v>
+        <v>60.730394623066189</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="2"/>
-        <v>10331.261733097697</v>
+        <v>10325.022443592001</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -675,18 +693,18 @@
       </c>
       <c r="C14" s="4">
         <f t="shared" si="0"/>
-        <v>10331.261733097697</v>
+        <v>10325.022443592001</v>
       </c>
       <c r="D14" s="4">
         <v>1000</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="1"/>
-        <v>67.043298587494704</v>
+        <v>67.006382791252662</v>
       </c>
       <c r="F14" s="4">
         <f t="shared" si="2"/>
-        <v>11398.305031685191</v>
+        <v>11392.028826383254</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -695,18 +713,18 @@
       </c>
       <c r="C15" s="4">
         <f t="shared" si="0"/>
-        <v>11398.305031685191</v>
+        <v>11392.028826383254</v>
       </c>
       <c r="D15" s="4">
         <v>1000</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="1"/>
-        <v>73.356638104137375</v>
+        <v>73.319503889434245</v>
       </c>
       <c r="F15" s="4">
         <f t="shared" si="2"/>
-        <v>12471.66166978933</v>
+        <v>12465.348330272687</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -715,18 +733,18 @@
       </c>
       <c r="C16" s="4">
         <f t="shared" si="0"/>
-        <v>12471.66166978933</v>
+        <v>12465.348330272687</v>
       </c>
       <c r="D16" s="4">
         <v>1000</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
-        <v>79.707331546253528</v>
+        <v>79.66997762078006</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="2"/>
-        <v>13551.369001335583</v>
+        <v>13545.018307893468</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -735,18 +753,18 @@
       </c>
       <c r="C17" s="4">
         <f t="shared" si="0"/>
-        <v>13551.369001335583</v>
+        <v>13545.018307893468</v>
       </c>
       <c r="D17" s="4">
         <v>1000</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="1"/>
-        <v>86.095599924568845</v>
+        <v>86.058024988369667</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="2"/>
-        <v>14637.464601260152</v>
+        <v>14631.076332881838</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -755,18 +773,18 @@
       </c>
       <c r="C18" s="4">
         <f t="shared" si="0"/>
-        <v>14637.464601260152</v>
+        <v>14631.076332881838</v>
       </c>
       <c r="D18" s="4">
         <v>1000</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="1"/>
-        <v>92.52166555745589</v>
+        <v>92.483868302884204</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="2"/>
-        <v>15729.986266817607</v>
+        <v>15723.560201184722</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -775,18 +793,18 @@
       </c>
       <c r="C19" s="4">
         <f t="shared" si="0"/>
-        <v>15729.986266817607</v>
+        <v>15723.560201184722</v>
       </c>
       <c r="D19" s="4">
         <v>1000</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="1"/>
-        <v>98.985752078670828</v>
+        <v>98.947731190342935</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="2"/>
-        <v>16828.972018896278</v>
+        <v>16822.507932375065</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -795,18 +813,18 @@
       </c>
       <c r="C20" s="4">
         <f t="shared" si="0"/>
-        <v>16828.972018896278</v>
+        <v>16822.507932375065</v>
       </c>
       <c r="D20" s="4">
         <v>1000</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="1"/>
-        <v>105.48808444513629</v>
+        <v>105.44983859988578</v>
       </c>
       <c r="F20" s="4">
         <f t="shared" si="2"/>
-        <v>17934.460103341415</v>
+        <v>17927.95777097495</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -815,34 +833,34 @@
       </c>
       <c r="C21" s="4">
         <f t="shared" si="0"/>
-        <v>17934.460103341415</v>
+        <v>17927.95777097495</v>
       </c>
       <c r="D21" s="4">
         <v>1000</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="1"/>
-        <v>112.02888894477003</v>
+        <v>111.99041681160178</v>
       </c>
       <c r="F21" s="4">
         <f t="shared" si="2"/>
-        <v>19046.488992286184</v>
+        <v>19039.948187786551</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C25">
         <v>1000</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>18</v>
@@ -850,7 +868,7 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="5">
         <v>7.0999999999999994E-2</v>
@@ -858,7 +876,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1">
         <f>FV(C27/12,C26,C25,,1)</f>
@@ -867,7 +885,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C34">
         <v>45000</v>
@@ -875,7 +893,7 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C35">
         <v>10</v>
@@ -883,7 +901,7 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C36" s="6">
         <v>0.08</v>
@@ -891,7 +909,7 @@
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" s="1">
         <f>FV(C36,C35,C34,,1)</f>
@@ -906,24 +924,281 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="7">
+        <f>SUM(D3*7.1%/12)</f>
+        <v>5.916666666666667</v>
+      </c>
+      <c r="F3" s="7">
+        <f>SUM(D3+E3)</f>
+        <v>1005.9166666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7">
+        <f>F3</f>
+        <v>1005.9166666666666</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="7">
+        <f>SUM((C4+D4)*7.1%/12)</f>
+        <v>11.868340277777776</v>
+      </c>
+      <c r="F4" s="7">
+        <f>SUM(C4+D4+E4)</f>
+        <v>2017.7850069444444</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" ref="C5:C14" si="0">F4</f>
+        <v>2017.7850069444444</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" ref="E5:E14" si="1">SUM((C5+D5)*7.1%/12)</f>
+        <v>17.855227957754629</v>
+      </c>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F14" si="2">SUM(C5+D5+E5)</f>
+        <v>3035.6402349021992</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>3035.6402349021992</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="1"/>
+        <v>23.877538056504676</v>
+      </c>
+      <c r="F6" s="7">
+        <f t="shared" si="2"/>
+        <v>4059.517772958704</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>4059.517772958704</v>
+      </c>
+      <c r="D7">
+        <v>1000</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="1"/>
+        <v>29.93548015667233</v>
+      </c>
+      <c r="F7" s="7">
+        <f t="shared" si="2"/>
+        <v>5089.4532531153764</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>5089.4532531153764</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>36.029265080932639</v>
+      </c>
+      <c r="F8" s="7">
+        <f t="shared" si="2"/>
+        <v>6125.4825181963088</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>6125.4825181963088</v>
+      </c>
+      <c r="D9">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="1"/>
+        <v>42.159104899328156</v>
+      </c>
+      <c r="F9" s="7">
+        <f t="shared" si="2"/>
+        <v>7167.6416230956365</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>7167.6416230956365</v>
+      </c>
+      <c r="D10">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
+        <v>48.325212936649173</v>
+      </c>
+      <c r="F10" s="7">
+        <f t="shared" si="2"/>
+        <v>8215.9668360322848</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>8215.9668360322848</v>
+      </c>
+      <c r="D11">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="1"/>
+        <v>54.527803779857685</v>
+      </c>
+      <c r="F11" s="7">
+        <f t="shared" si="2"/>
+        <v>9270.4946398121429</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>9270.4946398121429</v>
+      </c>
+      <c r="D12">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="1"/>
+        <v>60.767093285555177</v>
+      </c>
+      <c r="F12" s="7">
+        <f t="shared" si="2"/>
+        <v>10331.261733097697</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>10331.261733097697</v>
+      </c>
+      <c r="D13">
+        <v>1000</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="1"/>
+        <v>67.043298587494704</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="2"/>
+        <v>11398.305031685191</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="0"/>
+        <v>11398.305031685191</v>
+      </c>
+      <c r="D14">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="1"/>
+        <v>73.356638104137375</v>
+      </c>
+      <c r="F14" s="7">
+        <f t="shared" si="2"/>
+        <v>12471.66166978933</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>